<commit_message>
feat : 대화 나가기버튼 추가, docs : dialogSheet 수정
</commit_message>
<xml_diff>
--- a/URPRagProjectSingle/Assets/Characters/Skills/DataSheet/DialogData.xlsx
+++ b/URPRagProjectSingle/Assets/Characters/Skills/DataSheet/DialogData.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>type</t>
   </si>
@@ -120,6 +120,15 @@
   </si>
   <si>
     <t>나를 닮아 아주 잘 생겼지..</t>
+  </si>
+  <si>
+    <t>작별</t>
+  </si>
+  <si>
+    <t>이런 내가 너무 오래 잡아둔건가</t>
+  </si>
+  <si>
+    <t>즐거운 모험 되시게</t>
   </si>
 </sst>
 </file>
@@ -442,7 +451,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -457,7 +465,6 @@
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
       <left/>
@@ -466,7 +473,6 @@
       <bottom style="thick">
         <color theme="4"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
       <left/>
@@ -475,7 +481,6 @@
       <bottom style="thick">
         <color rgb="FFACCCEA"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
       <left/>
@@ -484,7 +489,6 @@
       <bottom style="medium">
         <color theme="4" tint="0.399980"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -499,7 +503,6 @@
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -514,7 +517,6 @@
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
       <left style="double">
@@ -529,7 +531,6 @@
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
       <left/>
@@ -538,7 +539,6 @@
       <bottom style="double">
         <color rgb="FFFF8001"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
       <left/>
@@ -549,7 +549,6 @@
       <bottom style="double">
         <color theme="4"/>
       </bottom>
-      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
@@ -1023,10 +1022,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.500000"/>
@@ -1261,16 +1260,50 @@
         <v>31</v>
       </c>
     </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="0">
+        <v>0</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="E13" s="0" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="0">
+        <v>1</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="E14" s="0" t="s">
+        <v>34</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A3:A4 A8 A14:A1048576 A5 A6 A7 A9 A10 A2 A11 A12 A13">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A3:A4 A8 A15:A1048576 A5 A6 A7 A9 A10 A2 A11 A12 A13 A14">
       <formula1>"dialog,greeting,leaveTalk,quest"</formula1>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1">
       <formula1>dialog,greeting,leaveTalk,quest</formula1>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C4 C8 C14:C1048576 C5 C6 C7 C2 C9 C10 C11 C12 C13">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C4 C8 C15:C1048576 C5 C6 C7 C2 C9 C10 C11 C12 C13 C14">
       <formula1>-2,147,483,648</formula1>
       <formula2>2,147,483,647</formula2>
     </dataValidation>

</xml_diff>